<commit_message>
changes made closer to finale
</commit_message>
<xml_diff>
--- a/pipline/sigmas.xlsx
+++ b/pipline/sigmas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WoomBat\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WoomBat\source\repos\Woombat84\WNA\pipline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313AF56A-550C-4A26-BBEF-2BC81634CAFC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDE3656-4372-4A4C-AEBC-62FE18A5702E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{A8BE0CD1-F75C-4648-A86C-9D68FC2513E9}"/>
   </bookViews>
@@ -97,12 +97,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,9 +147,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,7 +473,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,16 +530,16 @@
       <c r="G2">
         <v>36</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="2">
         <f>C2+(D2*K2)</f>
-        <v>39.588999999999999</v>
-      </c>
-      <c r="I2">
+        <v>42.76</v>
+      </c>
+      <c r="I2" s="2">
         <f>C2-(D2*K2)</f>
-        <v>33.247</v>
+        <v>30.076000000000001</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -525,16 +561,16 @@
       <c r="G3">
         <v>49</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="3">
         <f t="shared" ref="H3:H19" si="0">C3+(D3*K3)</f>
-        <v>57.265000000000001</v>
-      </c>
-      <c r="I3">
+        <v>62.833999999999996</v>
+      </c>
+      <c r="I3" s="3">
         <f t="shared" ref="I3:I19" si="1">C3-(D3*K3)</f>
-        <v>46.126999999999995</v>
+        <v>40.558</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -556,16 +592,16 @@
       <c r="G4">
         <v>103</v>
       </c>
-      <c r="H4" s="1">
-        <f t="shared" si="0"/>
-        <v>110.947</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="1"/>
-        <v>92.092999999999989</v>
+      <c r="H4" s="3">
+        <f t="shared" si="0"/>
+        <v>120.374</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="1"/>
+        <v>82.665999999999997</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -590,16 +626,16 @@
       <c r="G5">
         <v>58</v>
       </c>
-      <c r="H5" s="1">
-        <f t="shared" si="0"/>
-        <v>59.457999999999998</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="1"/>
-        <v>57.638000000000005</v>
+      <c r="H5" s="4">
+        <f t="shared" si="0"/>
+        <v>60.368000000000002</v>
+      </c>
+      <c r="I5" s="4">
+        <f>C5-(D5*K5)</f>
+        <v>56.728000000000002</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -621,16 +657,16 @@
       <c r="G6">
         <v>153</v>
       </c>
-      <c r="H6" s="1">
-        <f t="shared" si="0"/>
-        <v>163.18899999999999</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
-        <v>147.559</v>
+      <c r="H6" s="3">
+        <f t="shared" si="0"/>
+        <v>171.00399999999999</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="1"/>
+        <v>139.744</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -652,16 +688,16 @@
       <c r="G7">
         <v>107</v>
       </c>
-      <c r="H7" s="1">
-        <f t="shared" si="0"/>
-        <v>111.512</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
-        <v>100.82400000000001</v>
+      <c r="H7" s="3">
+        <f t="shared" si="0"/>
+        <v>116.85600000000001</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="1"/>
+        <v>95.48</v>
       </c>
       <c r="K7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -686,16 +722,16 @@
       <c r="G8">
         <v>60</v>
       </c>
-      <c r="H8" s="1">
-        <f t="shared" si="0"/>
-        <v>60.803000000000004</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="1"/>
-        <v>57.280999999999999</v>
+      <c r="H8" s="5">
+        <f t="shared" si="0"/>
+        <v>62.564</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" si="1"/>
+        <v>55.52</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -717,16 +753,16 @@
       <c r="G9">
         <v>162</v>
       </c>
-      <c r="H9" s="1">
-        <f t="shared" si="0"/>
-        <v>172.571</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="1"/>
-        <v>131.07300000000001</v>
+      <c r="H9" s="3">
+        <f t="shared" si="0"/>
+        <v>193.32</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="1"/>
+        <v>110.32400000000001</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -748,16 +784,16 @@
       <c r="G10">
         <v>88</v>
       </c>
-      <c r="H10" s="1">
-        <f t="shared" si="0"/>
-        <v>89.334000000000003</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="1"/>
-        <v>73.972000000000008</v>
+      <c r="H10" s="3">
+        <f t="shared" si="0"/>
+        <v>97.015000000000001</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" si="1"/>
+        <v>66.291000000000011</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -782,16 +818,16 @@
       <c r="G11">
         <v>45</v>
       </c>
-      <c r="H11" s="1">
-        <f t="shared" si="0"/>
-        <v>49.323999999999998</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
-        <v>43.456000000000003</v>
+      <c r="H11" s="6">
+        <f t="shared" si="0"/>
+        <v>52.258000000000003</v>
+      </c>
+      <c r="I11" s="6">
+        <f t="shared" si="1"/>
+        <v>40.521999999999998</v>
       </c>
       <c r="K11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -813,16 +849,16 @@
       <c r="G12">
         <v>170</v>
       </c>
-      <c r="H12" s="1">
-        <f t="shared" si="0"/>
-        <v>177.66800000000001</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="1"/>
-        <v>156.452</v>
+      <c r="H12" s="3">
+        <f t="shared" si="0"/>
+        <v>188.27600000000001</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" si="1"/>
+        <v>145.84399999999999</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -844,16 +880,16 @@
       <c r="G13">
         <v>179</v>
       </c>
-      <c r="H13" s="1">
-        <f t="shared" si="0"/>
-        <v>173.49599999999998</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="1"/>
-        <v>128.21600000000001</v>
+      <c r="H13" s="3">
+        <f t="shared" si="0"/>
+        <v>196.136</v>
+      </c>
+      <c r="I13" s="3">
+        <f t="shared" si="1"/>
+        <v>105.57599999999999</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -878,12 +914,12 @@
       <c r="G14">
         <v>8</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="7">
         <f t="shared" si="0"/>
         <v>89.957000000000008</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="1"/>
+      <c r="I14" s="7">
+        <f>C14-(D14*K14)</f>
         <v>-33.088999999999999</v>
       </c>
       <c r="K14">
@@ -909,11 +945,11 @@
       <c r="G15">
         <v>17</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="3">
         <f t="shared" si="0"/>
         <v>24.271000000000001</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="3">
         <f t="shared" si="1"/>
         <v>14.970999999999998</v>
       </c>
@@ -940,11 +976,11 @@
       <c r="G16">
         <v>76</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="3">
         <f t="shared" si="0"/>
         <v>82.088999999999999</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="3">
         <f t="shared" si="1"/>
         <v>67.676999999999992</v>
       </c>
@@ -974,11 +1010,11 @@
       <c r="G17">
         <v>240</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="7">
         <f t="shared" si="0"/>
         <v>287.76</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="7">
         <f t="shared" si="1"/>
         <v>140.28399999999999</v>
       </c>
@@ -1005,11 +1041,11 @@
       <c r="G18">
         <v>52</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="3">
         <f t="shared" si="0"/>
         <v>30.751000000000001</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="3">
         <f t="shared" si="1"/>
         <v>18.187000000000001</v>
       </c>
@@ -1036,11 +1072,11 @@
       <c r="G19">
         <v>58</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="3">
         <f t="shared" si="0"/>
         <v>66.411000000000001</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="3">
         <f t="shared" si="1"/>
         <v>53.319000000000003</v>
       </c>
@@ -1050,5 +1086,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>